<commit_message>
Added Fspar-Liq matching capabilities
</commit_message>
<xml_diff>
--- a/docs/Examples/Feldspar_Thermobarometry/Feldspar_Liquid.xlsx
+++ b/docs/Examples/Feldspar_Thermobarometry/Feldspar_Liquid.xlsx
@@ -1,22 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://oregonstateuniversity-my.sharepoint.com/personal/wieserp_oregonstate_edu/Documents/Postdoc/PyMME/MyBarometers/Thermobar_outer/Examples/Feldspar_Thermobarometry/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\penny\OneDrive - Oregon State University\Postdoc\PyMME\MyBarometers\Thermobar_outer\docs\Examples\Feldspar_Thermobarometry\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5E4CC164-538B-41A3-B286-E41F04A8C62A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBCA75C5-35AE-49C4-8929-6B717FF9D7FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="21840" windowHeight="13290" activeTab="1" xr2:uid="{A1311C21-BA00-45BD-8762-4D9CB1806536}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="21840" windowHeight="13290" activeTab="5" xr2:uid="{A1311C21-BA00-45BD-8762-4D9CB1806536}"/>
   </bookViews>
   <sheets>
     <sheet name="Plag_Liquid" sheetId="1" r:id="rId1"/>
     <sheet name="Kspar_Liquid" sheetId="2" r:id="rId2"/>
+    <sheet name="Plag_only" sheetId="3" r:id="rId3"/>
+    <sheet name="Liq_only" sheetId="4" r:id="rId4"/>
+    <sheet name="Kspar_only" sheetId="5" r:id="rId5"/>
+    <sheet name="Evolved_Liq_only" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="191029" iterate="1" iterateCount="500"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="104">
   <si>
     <t>Sample</t>
   </si>
@@ -137,13 +141,223 @@
   </si>
   <si>
     <t>Cr2O3_Kspar</t>
+  </si>
+  <si>
+    <t>Sample_ID_Plag</t>
+  </si>
+  <si>
+    <t>Plag1</t>
+  </si>
+  <si>
+    <t>Plag2</t>
+  </si>
+  <si>
+    <t>Plag3_core</t>
+  </si>
+  <si>
+    <t>Plag4</t>
+  </si>
+  <si>
+    <t>Plag5</t>
+  </si>
+  <si>
+    <t>Plag6</t>
+  </si>
+  <si>
+    <t>Plag7</t>
+  </si>
+  <si>
+    <t>Plag8</t>
+  </si>
+  <si>
+    <t>Plag9</t>
+  </si>
+  <si>
+    <t>Plag10</t>
+  </si>
+  <si>
+    <t>Plag11</t>
+  </si>
+  <si>
+    <t>Plag12</t>
+  </si>
+  <si>
+    <t>Plag13</t>
+  </si>
+  <si>
+    <t>Plag14</t>
+  </si>
+  <si>
+    <t>Plag15</t>
+  </si>
+  <si>
+    <t>Plag16</t>
+  </si>
+  <si>
+    <t>Plag17</t>
+  </si>
+  <si>
+    <t>Plag18</t>
+  </si>
+  <si>
+    <t>Plag19</t>
+  </si>
+  <si>
+    <t>Plag20</t>
+  </si>
+  <si>
+    <t>Plag21</t>
+  </si>
+  <si>
+    <t>Plag22</t>
+  </si>
+  <si>
+    <t>Plag23</t>
+  </si>
+  <si>
+    <t>Plag24</t>
+  </si>
+  <si>
+    <t>Plag25</t>
+  </si>
+  <si>
+    <t>Plag26</t>
+  </si>
+  <si>
+    <t>Plag27</t>
+  </si>
+  <si>
+    <t>Plag28</t>
+  </si>
+  <si>
+    <t>Sample_ID_Liq</t>
+  </si>
+  <si>
+    <t>Glass1</t>
+  </si>
+  <si>
+    <t>Glass2</t>
+  </si>
+  <si>
+    <t>Glass3</t>
+  </si>
+  <si>
+    <t>Glass4</t>
+  </si>
+  <si>
+    <t>Glass5</t>
+  </si>
+  <si>
+    <t>Glass6</t>
+  </si>
+  <si>
+    <t>Glass7</t>
+  </si>
+  <si>
+    <t>Glass8</t>
+  </si>
+  <si>
+    <t>Glass9</t>
+  </si>
+  <si>
+    <t>Glass10</t>
+  </si>
+  <si>
+    <t>Glass11</t>
+  </si>
+  <si>
+    <t>Glass12</t>
+  </si>
+  <si>
+    <t>Glass13</t>
+  </si>
+  <si>
+    <t>Glass14</t>
+  </si>
+  <si>
+    <t>Glass15</t>
+  </si>
+  <si>
+    <t>Glass16</t>
+  </si>
+  <si>
+    <t>Glass17</t>
+  </si>
+  <si>
+    <t>Glass18</t>
+  </si>
+  <si>
+    <t>Glass19</t>
+  </si>
+  <si>
+    <t>Glass20</t>
+  </si>
+  <si>
+    <t>Glass21</t>
+  </si>
+  <si>
+    <t>Glass22</t>
+  </si>
+  <si>
+    <t>Glass23</t>
+  </si>
+  <si>
+    <t>Glass24</t>
+  </si>
+  <si>
+    <t>Sample_ID_Kspar</t>
+  </si>
+  <si>
+    <t>Kspar1</t>
+  </si>
+  <si>
+    <t>Kspar2</t>
+  </si>
+  <si>
+    <t>Kspar3</t>
+  </si>
+  <si>
+    <t>Kspar4</t>
+  </si>
+  <si>
+    <t>Kspar5</t>
+  </si>
+  <si>
+    <t>Kspar6</t>
+  </si>
+  <si>
+    <t>Kspar7</t>
+  </si>
+  <si>
+    <t>Kspar8</t>
+  </si>
+  <si>
+    <t>Kspar9</t>
+  </si>
+  <si>
+    <t>Kspar10</t>
+  </si>
+  <si>
+    <t>Kspar11</t>
+  </si>
+  <si>
+    <t>Kspar12</t>
+  </si>
+  <si>
+    <t>Kspar13</t>
+  </si>
+  <si>
+    <t>Kspar14</t>
+  </si>
+  <si>
+    <t>Kspar15</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -162,6 +376,12 @@
       <sz val="10"/>
       <name val="Verdana"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -530,7 +750,7 @@
   <dimension ref="A1:X29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:X29"/>
+      <selection activeCell="L1" sqref="B1:L1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2634,8 +2854,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{333E94BA-3E45-4743-A9AA-8189ACA87F7B}">
   <dimension ref="A1:X16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:X16"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3680,4 +3900,3105 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65A02A0B-47E3-43D2-991D-5CE4065FBD97}">
+  <dimension ref="A1:K29"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:A29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:11" ht="28.2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="4">
+        <v>57.3</v>
+      </c>
+      <c r="C2" s="4">
+        <v>0.09</v>
+      </c>
+      <c r="D2" s="4">
+        <v>26.6</v>
+      </c>
+      <c r="E2" s="4">
+        <v>0.43</v>
+      </c>
+      <c r="F2" s="4">
+        <v>0</v>
+      </c>
+      <c r="G2" s="4">
+        <v>0.03</v>
+      </c>
+      <c r="H2" s="4">
+        <v>8.33</v>
+      </c>
+      <c r="I2" s="4">
+        <v>6.11</v>
+      </c>
+      <c r="J2" s="4">
+        <v>0.49</v>
+      </c>
+      <c r="K2" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="4">
+        <v>56.5</v>
+      </c>
+      <c r="C3" s="4">
+        <v>0.12</v>
+      </c>
+      <c r="D3" s="4">
+        <v>26.9</v>
+      </c>
+      <c r="E3" s="4">
+        <v>0.47</v>
+      </c>
+      <c r="F3" s="4">
+        <v>0</v>
+      </c>
+      <c r="G3" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="H3" s="4">
+        <v>8.9499999999999993</v>
+      </c>
+      <c r="I3" s="4">
+        <v>5.66</v>
+      </c>
+      <c r="J3" s="4">
+        <v>0.47</v>
+      </c>
+      <c r="K3" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="4">
+        <v>57.6</v>
+      </c>
+      <c r="C4" s="4">
+        <v>0.11</v>
+      </c>
+      <c r="D4" s="4">
+        <v>26.3</v>
+      </c>
+      <c r="E4" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="F4" s="4">
+        <v>0</v>
+      </c>
+      <c r="G4" s="4">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="H4" s="4">
+        <v>8.5</v>
+      </c>
+      <c r="I4" s="4">
+        <v>6.27</v>
+      </c>
+      <c r="J4" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="K4" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="4">
+        <v>57.2</v>
+      </c>
+      <c r="C5" s="4">
+        <v>0.16</v>
+      </c>
+      <c r="D5" s="4">
+        <v>27</v>
+      </c>
+      <c r="E5" s="4">
+        <v>0.62</v>
+      </c>
+      <c r="F5" s="4">
+        <v>0</v>
+      </c>
+      <c r="G5" s="4">
+        <v>0.06</v>
+      </c>
+      <c r="H5" s="4">
+        <v>9.0299999999999994</v>
+      </c>
+      <c r="I5" s="4">
+        <v>5.58</v>
+      </c>
+      <c r="J5" s="4">
+        <v>0.84</v>
+      </c>
+      <c r="K5" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="4">
+        <v>56.7</v>
+      </c>
+      <c r="C6" s="4">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="D6" s="4">
+        <v>27.6</v>
+      </c>
+      <c r="E6" s="4">
+        <v>0.69</v>
+      </c>
+      <c r="F6" s="4">
+        <v>0</v>
+      </c>
+      <c r="G6" s="4">
+        <v>0.11</v>
+      </c>
+      <c r="H6" s="4">
+        <v>9.4600000000000009</v>
+      </c>
+      <c r="I6" s="4">
+        <v>5.58</v>
+      </c>
+      <c r="J6" s="4">
+        <v>0.48</v>
+      </c>
+      <c r="K6" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="4">
+        <v>56</v>
+      </c>
+      <c r="C7" s="4">
+        <v>0.21</v>
+      </c>
+      <c r="D7" s="4">
+        <v>26.6</v>
+      </c>
+      <c r="E7" s="4">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="F7" s="4">
+        <v>0</v>
+      </c>
+      <c r="G7" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="H7" s="4">
+        <v>8.99</v>
+      </c>
+      <c r="I7" s="4">
+        <v>5.7</v>
+      </c>
+      <c r="J7" s="4">
+        <v>0.45</v>
+      </c>
+      <c r="K7" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" s="4">
+        <v>56.1</v>
+      </c>
+      <c r="C8" s="4">
+        <v>0.21</v>
+      </c>
+      <c r="D8" s="4">
+        <v>27.8</v>
+      </c>
+      <c r="E8" s="4">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="F8" s="4">
+        <v>0</v>
+      </c>
+      <c r="G8" s="4">
+        <v>0.09</v>
+      </c>
+      <c r="H8" s="4">
+        <v>9.94</v>
+      </c>
+      <c r="I8" s="4">
+        <v>5.53</v>
+      </c>
+      <c r="J8" s="4">
+        <v>0.38</v>
+      </c>
+      <c r="K8" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" s="4">
+        <v>56.4</v>
+      </c>
+      <c r="C9" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="D9" s="4">
+        <v>27.3</v>
+      </c>
+      <c r="E9" s="4">
+        <v>0.53</v>
+      </c>
+      <c r="F9" s="4">
+        <v>0</v>
+      </c>
+      <c r="G9" s="4">
+        <v>0.08</v>
+      </c>
+      <c r="H9" s="4">
+        <v>9.61</v>
+      </c>
+      <c r="I9" s="4">
+        <v>5.48</v>
+      </c>
+      <c r="J9" s="4">
+        <v>0.36</v>
+      </c>
+      <c r="K9" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" s="4">
+        <v>56</v>
+      </c>
+      <c r="C10" s="4">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="D10" s="4">
+        <v>27</v>
+      </c>
+      <c r="E10" s="4">
+        <v>0.64</v>
+      </c>
+      <c r="F10" s="4">
+        <v>0</v>
+      </c>
+      <c r="G10" s="4">
+        <v>0.09</v>
+      </c>
+      <c r="H10" s="4">
+        <v>9.68</v>
+      </c>
+      <c r="I10" s="4">
+        <v>5.26</v>
+      </c>
+      <c r="J10" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="K10" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" s="4">
+        <v>54.5</v>
+      </c>
+      <c r="C11" s="4">
+        <v>0</v>
+      </c>
+      <c r="D11" s="4">
+        <v>27.5</v>
+      </c>
+      <c r="E11" s="4">
+        <v>0.75</v>
+      </c>
+      <c r="F11" s="4">
+        <v>0</v>
+      </c>
+      <c r="G11" s="4">
+        <v>0.24</v>
+      </c>
+      <c r="H11" s="4">
+        <v>11.1</v>
+      </c>
+      <c r="I11" s="4">
+        <v>4.74</v>
+      </c>
+      <c r="J11" s="4">
+        <v>0.35</v>
+      </c>
+      <c r="K11" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" s="4">
+        <v>53.8</v>
+      </c>
+      <c r="C12" s="4">
+        <v>0</v>
+      </c>
+      <c r="D12" s="4">
+        <v>28.3</v>
+      </c>
+      <c r="E12" s="4">
+        <v>0.67</v>
+      </c>
+      <c r="F12" s="4">
+        <v>0</v>
+      </c>
+      <c r="G12" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="H12" s="4">
+        <v>11.9</v>
+      </c>
+      <c r="I12" s="4">
+        <v>4.45</v>
+      </c>
+      <c r="J12" s="4">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="K12" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" s="4">
+        <v>54.1</v>
+      </c>
+      <c r="C13" s="4">
+        <v>0</v>
+      </c>
+      <c r="D13" s="4">
+        <v>28.8</v>
+      </c>
+      <c r="E13" s="4">
+        <v>0.75</v>
+      </c>
+      <c r="F13" s="4">
+        <v>0</v>
+      </c>
+      <c r="G13" s="4">
+        <v>0.22</v>
+      </c>
+      <c r="H13" s="4">
+        <v>11.9</v>
+      </c>
+      <c r="I13" s="4">
+        <v>4.34</v>
+      </c>
+      <c r="J13" s="4">
+        <v>0.25</v>
+      </c>
+      <c r="K13" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14" s="4">
+        <v>51.98</v>
+      </c>
+      <c r="C14" s="4">
+        <v>0.12</v>
+      </c>
+      <c r="D14" s="4">
+        <v>29.3</v>
+      </c>
+      <c r="E14" s="4">
+        <v>0.61</v>
+      </c>
+      <c r="F14" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="G14" s="4">
+        <v>0.21</v>
+      </c>
+      <c r="H14" s="4">
+        <v>12.84</v>
+      </c>
+      <c r="I14" s="4">
+        <v>4.03</v>
+      </c>
+      <c r="J14" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="K14" s="4"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15" s="4">
+        <v>52.89</v>
+      </c>
+      <c r="C15" s="4">
+        <v>0.13</v>
+      </c>
+      <c r="D15" s="4">
+        <v>28.38</v>
+      </c>
+      <c r="E15" s="4">
+        <v>1.19</v>
+      </c>
+      <c r="F15" s="4">
+        <v>0.03</v>
+      </c>
+      <c r="G15" s="4">
+        <v>0.83</v>
+      </c>
+      <c r="H15" s="4">
+        <v>12</v>
+      </c>
+      <c r="I15" s="4">
+        <v>4.04</v>
+      </c>
+      <c r="J15" s="4">
+        <v>0.45</v>
+      </c>
+      <c r="K15" s="4"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>49</v>
+      </c>
+      <c r="B16" s="4">
+        <v>49.98</v>
+      </c>
+      <c r="C16" s="4">
+        <v>0.09</v>
+      </c>
+      <c r="D16" s="4">
+        <v>31.6</v>
+      </c>
+      <c r="E16" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="F16" s="4">
+        <v>0</v>
+      </c>
+      <c r="G16" s="4">
+        <v>0.22</v>
+      </c>
+      <c r="H16" s="4">
+        <v>14.4</v>
+      </c>
+      <c r="I16" s="4">
+        <v>3.1110000000000002</v>
+      </c>
+      <c r="J16" s="4">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="K16" s="4"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>50</v>
+      </c>
+      <c r="B17" s="4">
+        <v>51.58</v>
+      </c>
+      <c r="C17" s="4">
+        <v>0.13</v>
+      </c>
+      <c r="D17" s="4">
+        <v>30.48</v>
+      </c>
+      <c r="E17" s="4">
+        <v>0.81</v>
+      </c>
+      <c r="F17" s="4">
+        <v>0</v>
+      </c>
+      <c r="G17" s="4">
+        <v>0.25</v>
+      </c>
+      <c r="H17" s="4">
+        <v>13.7</v>
+      </c>
+      <c r="I17" s="4">
+        <v>3.43</v>
+      </c>
+      <c r="J17" s="4">
+        <v>0.19</v>
+      </c>
+      <c r="K17" s="4"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>51</v>
+      </c>
+      <c r="B18" s="4">
+        <v>51.96</v>
+      </c>
+      <c r="C18" s="4">
+        <v>0.15</v>
+      </c>
+      <c r="D18" s="4">
+        <v>29.49</v>
+      </c>
+      <c r="E18" s="4">
+        <v>0.74</v>
+      </c>
+      <c r="F18" s="4">
+        <v>0</v>
+      </c>
+      <c r="G18" s="4">
+        <v>0.41</v>
+      </c>
+      <c r="H18" s="4">
+        <v>12.91</v>
+      </c>
+      <c r="I18" s="4">
+        <v>3.77</v>
+      </c>
+      <c r="J18" s="4">
+        <v>0.26</v>
+      </c>
+      <c r="K18" s="4"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>52</v>
+      </c>
+      <c r="B19" s="4">
+        <v>52.25</v>
+      </c>
+      <c r="C19" s="4">
+        <v>0.18</v>
+      </c>
+      <c r="D19" s="4">
+        <v>28.96</v>
+      </c>
+      <c r="E19" s="4">
+        <v>0.8</v>
+      </c>
+      <c r="F19" s="4">
+        <v>0</v>
+      </c>
+      <c r="G19" s="4">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="H19" s="4">
+        <v>12.67</v>
+      </c>
+      <c r="I19" s="4">
+        <v>3.95</v>
+      </c>
+      <c r="J19" s="4">
+        <v>0.35</v>
+      </c>
+      <c r="K19" s="4"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>53</v>
+      </c>
+      <c r="B20" s="4">
+        <v>52.78</v>
+      </c>
+      <c r="C20" s="4">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="D20" s="4">
+        <v>28.29</v>
+      </c>
+      <c r="E20" s="4">
+        <v>0.74</v>
+      </c>
+      <c r="F20" s="4">
+        <v>0.02</v>
+      </c>
+      <c r="G20" s="4">
+        <v>0.18</v>
+      </c>
+      <c r="H20" s="4">
+        <v>11.65</v>
+      </c>
+      <c r="I20" s="4">
+        <v>4.53</v>
+      </c>
+      <c r="J20" s="4">
+        <v>0.54</v>
+      </c>
+      <c r="K20" s="4"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>54</v>
+      </c>
+      <c r="B21" s="4">
+        <v>48.73</v>
+      </c>
+      <c r="C21" s="4">
+        <v>0.06</v>
+      </c>
+      <c r="D21" s="4">
+        <v>31.46</v>
+      </c>
+      <c r="E21" s="4">
+        <v>0.35</v>
+      </c>
+      <c r="F21" s="4">
+        <v>0</v>
+      </c>
+      <c r="G21" s="4">
+        <v>0.22</v>
+      </c>
+      <c r="H21" s="4">
+        <v>15.41</v>
+      </c>
+      <c r="I21" s="4">
+        <v>2.6</v>
+      </c>
+      <c r="J21" s="4">
+        <v>0.09</v>
+      </c>
+      <c r="K21" s="4"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>55</v>
+      </c>
+      <c r="B22" s="4">
+        <v>50.14</v>
+      </c>
+      <c r="C22" s="4">
+        <v>0.08</v>
+      </c>
+      <c r="D22" s="4">
+        <v>30.58</v>
+      </c>
+      <c r="E22" s="4">
+        <v>0.35</v>
+      </c>
+      <c r="F22" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="G22" s="4">
+        <v>0.25</v>
+      </c>
+      <c r="H22" s="4">
+        <v>14.7</v>
+      </c>
+      <c r="I22" s="4">
+        <v>3.05</v>
+      </c>
+      <c r="J22" s="4">
+        <v>0.11</v>
+      </c>
+      <c r="K22" s="4"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>56</v>
+      </c>
+      <c r="B23" s="4">
+        <v>51.45</v>
+      </c>
+      <c r="C23" s="4">
+        <v>0.11</v>
+      </c>
+      <c r="D23" s="4">
+        <v>30.05</v>
+      </c>
+      <c r="E23" s="4">
+        <v>0.51</v>
+      </c>
+      <c r="F23" s="4">
+        <v>0</v>
+      </c>
+      <c r="G23" s="4">
+        <v>0.23</v>
+      </c>
+      <c r="H23" s="4">
+        <v>13.83</v>
+      </c>
+      <c r="I23" s="4">
+        <v>3.53</v>
+      </c>
+      <c r="J23" s="4">
+        <v>0.17</v>
+      </c>
+      <c r="K23" s="4"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>57</v>
+      </c>
+      <c r="B24" s="4">
+        <v>52.17</v>
+      </c>
+      <c r="C24" s="4">
+        <v>0.13</v>
+      </c>
+      <c r="D24" s="4">
+        <v>29.58</v>
+      </c>
+      <c r="E24" s="4">
+        <v>0.66</v>
+      </c>
+      <c r="F24" s="4">
+        <v>0.03</v>
+      </c>
+      <c r="G24" s="4">
+        <v>0.23</v>
+      </c>
+      <c r="H24" s="4">
+        <v>13.23</v>
+      </c>
+      <c r="I24" s="4">
+        <v>3.78</v>
+      </c>
+      <c r="J24" s="4">
+        <v>0.25</v>
+      </c>
+      <c r="K24" s="4"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>58</v>
+      </c>
+      <c r="B25" s="4">
+        <v>53.35</v>
+      </c>
+      <c r="C25" s="4">
+        <v>0.23</v>
+      </c>
+      <c r="D25" s="4">
+        <v>28.83</v>
+      </c>
+      <c r="E25" s="4">
+        <v>0.83</v>
+      </c>
+      <c r="F25" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="G25" s="4">
+        <v>0.32</v>
+      </c>
+      <c r="H25" s="4">
+        <v>12.67</v>
+      </c>
+      <c r="I25" s="4">
+        <v>4.1100000000000003</v>
+      </c>
+      <c r="J25" s="4">
+        <v>0.32</v>
+      </c>
+      <c r="K25" s="4"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>59</v>
+      </c>
+      <c r="B26" s="4">
+        <v>54.4</v>
+      </c>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4">
+        <v>28.8</v>
+      </c>
+      <c r="E26" s="4">
+        <v>0.16</v>
+      </c>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4">
+        <v>0.06</v>
+      </c>
+      <c r="H26" s="4">
+        <v>11.05</v>
+      </c>
+      <c r="I26" s="4">
+        <v>4.84</v>
+      </c>
+      <c r="J26" s="4">
+        <v>0.11</v>
+      </c>
+      <c r="K26" s="4"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>60</v>
+      </c>
+      <c r="B27" s="4">
+        <v>53</v>
+      </c>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4">
+        <v>29.6</v>
+      </c>
+      <c r="E27" s="4">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4">
+        <v>0.03</v>
+      </c>
+      <c r="H27" s="4">
+        <v>12.67</v>
+      </c>
+      <c r="I27" s="4">
+        <v>4.45</v>
+      </c>
+      <c r="J27" s="4">
+        <v>0.08</v>
+      </c>
+      <c r="K27" s="4"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>61</v>
+      </c>
+      <c r="B28" s="4">
+        <v>54.1</v>
+      </c>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4">
+        <v>28.7</v>
+      </c>
+      <c r="E28" s="4">
+        <v>0.24</v>
+      </c>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4">
+        <v>0.02</v>
+      </c>
+      <c r="H28" s="4">
+        <v>11.46</v>
+      </c>
+      <c r="I28" s="4">
+        <v>4.97</v>
+      </c>
+      <c r="J28" s="4">
+        <v>0.11</v>
+      </c>
+      <c r="K28" s="4"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>62</v>
+      </c>
+      <c r="B29" s="4">
+        <v>54.5</v>
+      </c>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4">
+        <v>28.6</v>
+      </c>
+      <c r="E29" s="4">
+        <v>0.26</v>
+      </c>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4">
+        <v>0.03</v>
+      </c>
+      <c r="H29" s="4">
+        <v>11.38</v>
+      </c>
+      <c r="I29" s="4">
+        <v>4.95</v>
+      </c>
+      <c r="J29" s="4">
+        <v>0.12</v>
+      </c>
+      <c r="K29" s="4"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D836E083-7C8B-4ECA-81DC-C86CD23608AC}">
+  <dimension ref="A1:L29"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="20.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="28.2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="4">
+        <v>49.1</v>
+      </c>
+      <c r="C2" s="4">
+        <v>3.22</v>
+      </c>
+      <c r="D2" s="4">
+        <v>14.4</v>
+      </c>
+      <c r="E2" s="4">
+        <v>14.8</v>
+      </c>
+      <c r="F2" s="4">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="G2" s="4">
+        <v>3.2</v>
+      </c>
+      <c r="H2" s="4">
+        <v>6.72</v>
+      </c>
+      <c r="I2" s="4">
+        <v>3.34</v>
+      </c>
+      <c r="J2" s="4">
+        <v>1.7</v>
+      </c>
+      <c r="K2" s="4">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="L2" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3" s="4">
+        <v>49.2</v>
+      </c>
+      <c r="C3" s="4">
+        <v>3.89</v>
+      </c>
+      <c r="D3" s="4">
+        <v>15.3</v>
+      </c>
+      <c r="E3" s="4">
+        <v>13.7</v>
+      </c>
+      <c r="F3" s="4">
+        <v>0.12</v>
+      </c>
+      <c r="G3" s="4">
+        <v>3.88</v>
+      </c>
+      <c r="H3" s="4">
+        <v>6.76</v>
+      </c>
+      <c r="I3" s="4">
+        <v>3.44</v>
+      </c>
+      <c r="J3" s="4">
+        <v>1.22</v>
+      </c>
+      <c r="K3" s="4">
+        <v>0.83</v>
+      </c>
+      <c r="L3" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B4" s="4">
+        <v>49.6</v>
+      </c>
+      <c r="C4" s="4">
+        <v>3.79</v>
+      </c>
+      <c r="D4" s="4">
+        <v>15.8</v>
+      </c>
+      <c r="E4" s="4">
+        <v>13</v>
+      </c>
+      <c r="F4" s="4">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="G4" s="4">
+        <v>4.26</v>
+      </c>
+      <c r="H4" s="4">
+        <v>6.59</v>
+      </c>
+      <c r="I4" s="4">
+        <v>3.65</v>
+      </c>
+      <c r="J4" s="4">
+        <v>1.04</v>
+      </c>
+      <c r="K4" s="4">
+        <v>0.63</v>
+      </c>
+      <c r="L4" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5" s="4">
+        <v>47.1</v>
+      </c>
+      <c r="C5" s="4">
+        <v>4.21</v>
+      </c>
+      <c r="D5" s="4">
+        <v>12</v>
+      </c>
+      <c r="E5" s="4">
+        <v>17.8</v>
+      </c>
+      <c r="F5" s="4">
+        <v>0.18</v>
+      </c>
+      <c r="G5" s="4">
+        <v>3.4</v>
+      </c>
+      <c r="H5" s="4">
+        <v>7.28</v>
+      </c>
+      <c r="I5" s="4">
+        <v>2.93</v>
+      </c>
+      <c r="J5" s="4">
+        <v>2.02</v>
+      </c>
+      <c r="K5" s="4">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="L5" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B6" s="4">
+        <v>48.1</v>
+      </c>
+      <c r="C6" s="4">
+        <v>3.88</v>
+      </c>
+      <c r="D6" s="4">
+        <v>13.2</v>
+      </c>
+      <c r="E6" s="4">
+        <v>16.399999999999999</v>
+      </c>
+      <c r="F6" s="4">
+        <v>0.16</v>
+      </c>
+      <c r="G6" s="4">
+        <v>4.0199999999999996</v>
+      </c>
+      <c r="H6" s="4">
+        <v>6.51</v>
+      </c>
+      <c r="I6" s="4">
+        <v>3.36</v>
+      </c>
+      <c r="J6" s="4">
+        <v>1.36</v>
+      </c>
+      <c r="K6" s="4">
+        <v>1.59</v>
+      </c>
+      <c r="L6" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B7" s="4">
+        <v>48.2</v>
+      </c>
+      <c r="C7" s="4">
+        <v>4.8899999999999997</v>
+      </c>
+      <c r="D7" s="4">
+        <v>14.1</v>
+      </c>
+      <c r="E7" s="4">
+        <v>14.2</v>
+      </c>
+      <c r="F7" s="4">
+        <v>0.16</v>
+      </c>
+      <c r="G7" s="4">
+        <v>4.67</v>
+      </c>
+      <c r="H7" s="4">
+        <v>6.37</v>
+      </c>
+      <c r="I7" s="4">
+        <v>3.46</v>
+      </c>
+      <c r="J7" s="4">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="K7" s="4">
+        <v>0.79</v>
+      </c>
+      <c r="L7" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B8" s="4">
+        <v>49.5</v>
+      </c>
+      <c r="C8" s="4">
+        <v>4.2300000000000004</v>
+      </c>
+      <c r="D8" s="4">
+        <v>14.8</v>
+      </c>
+      <c r="E8" s="4">
+        <v>14</v>
+      </c>
+      <c r="F8" s="4">
+        <v>0.16</v>
+      </c>
+      <c r="G8" s="4">
+        <v>4.63</v>
+      </c>
+      <c r="H8" s="4">
+        <v>6.36</v>
+      </c>
+      <c r="I8" s="4">
+        <v>3.76</v>
+      </c>
+      <c r="J8" s="4">
+        <v>1.04</v>
+      </c>
+      <c r="K8" s="4">
+        <v>0.69</v>
+      </c>
+      <c r="L8" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>71</v>
+      </c>
+      <c r="B9" s="4">
+        <v>49.5</v>
+      </c>
+      <c r="C9" s="4">
+        <v>4.04</v>
+      </c>
+      <c r="D9" s="4">
+        <v>15.3</v>
+      </c>
+      <c r="E9" s="4">
+        <v>13.5</v>
+      </c>
+      <c r="F9" s="4">
+        <v>0.13</v>
+      </c>
+      <c r="G9" s="4">
+        <v>4.6500000000000004</v>
+      </c>
+      <c r="H9" s="4">
+        <v>6.39</v>
+      </c>
+      <c r="I9" s="4">
+        <v>3.62</v>
+      </c>
+      <c r="J9" s="4">
+        <v>0.9</v>
+      </c>
+      <c r="K9" s="4">
+        <v>0.66</v>
+      </c>
+      <c r="L9" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>72</v>
+      </c>
+      <c r="B10" s="4">
+        <v>52</v>
+      </c>
+      <c r="C10" s="4">
+        <v>4.04</v>
+      </c>
+      <c r="D10" s="4">
+        <v>12.5</v>
+      </c>
+      <c r="E10" s="4">
+        <v>14.3</v>
+      </c>
+      <c r="F10" s="4">
+        <v>0.15</v>
+      </c>
+      <c r="G10" s="4">
+        <v>3.3</v>
+      </c>
+      <c r="H10" s="4">
+        <v>6.71</v>
+      </c>
+      <c r="I10" s="4">
+        <v>2.8</v>
+      </c>
+      <c r="J10" s="4">
+        <v>1.41</v>
+      </c>
+      <c r="K10" s="4">
+        <v>1.17</v>
+      </c>
+      <c r="L10" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>73</v>
+      </c>
+      <c r="B11" s="4">
+        <v>57.8</v>
+      </c>
+      <c r="C11" s="4">
+        <v>1.87</v>
+      </c>
+      <c r="D11" s="4">
+        <v>13.7</v>
+      </c>
+      <c r="E11" s="4">
+        <v>9.35</v>
+      </c>
+      <c r="F11" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="G11" s="4">
+        <v>3.41</v>
+      </c>
+      <c r="H11" s="4">
+        <v>6.33</v>
+      </c>
+      <c r="I11" s="4">
+        <v>3.82</v>
+      </c>
+      <c r="J11" s="4">
+        <v>1.94</v>
+      </c>
+      <c r="K11" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="L11" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>74</v>
+      </c>
+      <c r="B12" s="4">
+        <v>57.9</v>
+      </c>
+      <c r="C12" s="4">
+        <v>1.77</v>
+      </c>
+      <c r="D12" s="4">
+        <v>13.8</v>
+      </c>
+      <c r="E12" s="4">
+        <v>9.4499999999999993</v>
+      </c>
+      <c r="F12" s="4">
+        <v>0.19</v>
+      </c>
+      <c r="G12" s="4">
+        <v>3.67</v>
+      </c>
+      <c r="H12" s="4">
+        <v>6.78</v>
+      </c>
+      <c r="I12" s="4">
+        <v>3.82</v>
+      </c>
+      <c r="J12" s="4">
+        <v>1.81</v>
+      </c>
+      <c r="K12" s="4">
+        <v>0.37</v>
+      </c>
+      <c r="L12" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>75</v>
+      </c>
+      <c r="B13" s="4">
+        <v>57.4</v>
+      </c>
+      <c r="C13" s="4">
+        <v>1.74</v>
+      </c>
+      <c r="D13" s="4">
+        <v>13.8</v>
+      </c>
+      <c r="E13" s="4">
+        <v>9.3800000000000008</v>
+      </c>
+      <c r="F13" s="4">
+        <v>0.21</v>
+      </c>
+      <c r="G13" s="4">
+        <v>3.99</v>
+      </c>
+      <c r="H13" s="4">
+        <v>6.8</v>
+      </c>
+      <c r="I13" s="4">
+        <v>3.62</v>
+      </c>
+      <c r="J13" s="4">
+        <v>1.69</v>
+      </c>
+      <c r="K13" s="4">
+        <v>0.31</v>
+      </c>
+      <c r="L13" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>76</v>
+      </c>
+      <c r="B14" s="4">
+        <v>45.38</v>
+      </c>
+      <c r="C14" s="4">
+        <v>3.24</v>
+      </c>
+      <c r="D14" s="4">
+        <v>14.03</v>
+      </c>
+      <c r="E14" s="4">
+        <v>13.85</v>
+      </c>
+      <c r="F14" s="4">
+        <v>0.22</v>
+      </c>
+      <c r="G14" s="4">
+        <v>5.35</v>
+      </c>
+      <c r="H14" s="4">
+        <v>9.48</v>
+      </c>
+      <c r="I14" s="4">
+        <v>3.2</v>
+      </c>
+      <c r="J14" s="4">
+        <v>1.07</v>
+      </c>
+      <c r="K14" s="4">
+        <v>0.59</v>
+      </c>
+      <c r="L14" s="4">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>77</v>
+      </c>
+      <c r="B15" s="4">
+        <v>44.48</v>
+      </c>
+      <c r="C15" s="4">
+        <v>5.66</v>
+      </c>
+      <c r="D15" s="4">
+        <v>12.9</v>
+      </c>
+      <c r="E15" s="4">
+        <v>14.96</v>
+      </c>
+      <c r="F15" s="4">
+        <v>0.26</v>
+      </c>
+      <c r="G15" s="4">
+        <v>4.95</v>
+      </c>
+      <c r="H15" s="4">
+        <v>9.11</v>
+      </c>
+      <c r="I15" s="4">
+        <v>2.82</v>
+      </c>
+      <c r="J15" s="4">
+        <v>1.56</v>
+      </c>
+      <c r="K15" s="4">
+        <v>1.19</v>
+      </c>
+      <c r="L15" s="4">
+        <v>0.37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>78</v>
+      </c>
+      <c r="B16" s="4">
+        <v>47.7</v>
+      </c>
+      <c r="C16" s="4">
+        <v>1.73</v>
+      </c>
+      <c r="D16" s="4">
+        <v>15.88</v>
+      </c>
+      <c r="E16" s="4">
+        <v>10.17</v>
+      </c>
+      <c r="F16" s="4">
+        <v>0.19</v>
+      </c>
+      <c r="G16" s="4">
+        <v>7</v>
+      </c>
+      <c r="H16" s="4">
+        <v>11.48</v>
+      </c>
+      <c r="I16" s="4">
+        <v>2.54</v>
+      </c>
+      <c r="J16" s="4">
+        <v>0.52</v>
+      </c>
+      <c r="K16" s="4">
+        <v>0.27</v>
+      </c>
+      <c r="L16" s="4">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>79</v>
+      </c>
+      <c r="B17" s="4">
+        <v>47.66</v>
+      </c>
+      <c r="C17" s="4">
+        <v>2.75</v>
+      </c>
+      <c r="D17" s="4">
+        <v>14.07</v>
+      </c>
+      <c r="E17" s="4">
+        <v>12.56</v>
+      </c>
+      <c r="F17" s="4">
+        <v>0.22</v>
+      </c>
+      <c r="G17" s="4">
+        <v>6</v>
+      </c>
+      <c r="H17" s="4">
+        <v>10.68</v>
+      </c>
+      <c r="I17" s="4">
+        <v>2.89</v>
+      </c>
+      <c r="J17" s="4">
+        <v>0.78</v>
+      </c>
+      <c r="K17" s="4">
+        <v>0.46</v>
+      </c>
+      <c r="L17" s="4">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>80</v>
+      </c>
+      <c r="B18" s="4">
+        <v>46.18</v>
+      </c>
+      <c r="C18" s="4">
+        <v>3.36</v>
+      </c>
+      <c r="D18" s="4">
+        <v>13.8</v>
+      </c>
+      <c r="E18" s="4">
+        <v>13.02</v>
+      </c>
+      <c r="F18" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="G18" s="4">
+        <v>5.23</v>
+      </c>
+      <c r="H18" s="4">
+        <v>9.91</v>
+      </c>
+      <c r="I18" s="4">
+        <v>3.05</v>
+      </c>
+      <c r="J18" s="4">
+        <v>1.04</v>
+      </c>
+      <c r="K18" s="4">
+        <v>0.67</v>
+      </c>
+      <c r="L18" s="4">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>81</v>
+      </c>
+      <c r="B19" s="4">
+        <v>45.99</v>
+      </c>
+      <c r="C19" s="4">
+        <v>4.33</v>
+      </c>
+      <c r="D19" s="4">
+        <v>13.34</v>
+      </c>
+      <c r="E19" s="4">
+        <v>13.69</v>
+      </c>
+      <c r="F19" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="G19" s="4">
+        <v>4.72</v>
+      </c>
+      <c r="H19" s="4">
+        <v>9.25</v>
+      </c>
+      <c r="I19" s="4">
+        <v>3.03</v>
+      </c>
+      <c r="J19" s="4">
+        <v>1.37</v>
+      </c>
+      <c r="K19" s="4">
+        <v>0.96</v>
+      </c>
+      <c r="L19" s="4">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>82</v>
+      </c>
+      <c r="B20" s="4">
+        <v>46.15</v>
+      </c>
+      <c r="C20" s="4">
+        <v>5.21</v>
+      </c>
+      <c r="D20" s="4">
+        <v>13.59</v>
+      </c>
+      <c r="E20" s="4">
+        <v>13.57</v>
+      </c>
+      <c r="F20" s="4">
+        <v>0.13</v>
+      </c>
+      <c r="G20" s="4">
+        <v>4.37</v>
+      </c>
+      <c r="H20" s="4">
+        <v>8.8800000000000008</v>
+      </c>
+      <c r="I20" s="4">
+        <v>3.05</v>
+      </c>
+      <c r="J20" s="4">
+        <v>1.8</v>
+      </c>
+      <c r="K20" s="4">
+        <v>1.18</v>
+      </c>
+      <c r="L20" s="4">
+        <v>0.42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>83</v>
+      </c>
+      <c r="B21" s="4">
+        <v>48.07</v>
+      </c>
+      <c r="C21" s="4">
+        <v>1.63</v>
+      </c>
+      <c r="D21" s="4">
+        <v>16.16</v>
+      </c>
+      <c r="E21" s="4">
+        <v>10.16</v>
+      </c>
+      <c r="F21" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="G21" s="4">
+        <v>7.72</v>
+      </c>
+      <c r="H21" s="4">
+        <v>11.39</v>
+      </c>
+      <c r="I21" s="4">
+        <v>2.57</v>
+      </c>
+      <c r="J21" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="K21" s="4">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="L21" s="4">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>84</v>
+      </c>
+      <c r="B22" s="4">
+        <v>47.81</v>
+      </c>
+      <c r="C22" s="4">
+        <v>1.89</v>
+      </c>
+      <c r="D22" s="4">
+        <v>14.86</v>
+      </c>
+      <c r="E22" s="4">
+        <v>10.91</v>
+      </c>
+      <c r="F22" s="4">
+        <v>0.16</v>
+      </c>
+      <c r="G22" s="4">
+        <v>7.01</v>
+      </c>
+      <c r="H22" s="4">
+        <v>11.58</v>
+      </c>
+      <c r="I22" s="4">
+        <v>2.66</v>
+      </c>
+      <c r="J22" s="4">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="K22" s="4">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="L22" s="4">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>85</v>
+      </c>
+      <c r="B23" s="4">
+        <v>47.79</v>
+      </c>
+      <c r="C23" s="4">
+        <v>2.85</v>
+      </c>
+      <c r="D23" s="4">
+        <v>13.95</v>
+      </c>
+      <c r="E23" s="4">
+        <v>12.55</v>
+      </c>
+      <c r="F23" s="4">
+        <v>0.17</v>
+      </c>
+      <c r="G23" s="4">
+        <v>5.73</v>
+      </c>
+      <c r="H23" s="4">
+        <v>10.72</v>
+      </c>
+      <c r="I23" s="4">
+        <v>3.07</v>
+      </c>
+      <c r="J23" s="4">
+        <v>0.88</v>
+      </c>
+      <c r="K23" s="4">
+        <v>0.52</v>
+      </c>
+      <c r="L23" s="4">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>86</v>
+      </c>
+      <c r="B24" s="4">
+        <v>47.35</v>
+      </c>
+      <c r="C24" s="4">
+        <v>3.42</v>
+      </c>
+      <c r="D24" s="4">
+        <v>13.37</v>
+      </c>
+      <c r="E24" s="4">
+        <v>13.41</v>
+      </c>
+      <c r="F24" s="4">
+        <v>0.22</v>
+      </c>
+      <c r="G24" s="4">
+        <v>5.18</v>
+      </c>
+      <c r="H24" s="4">
+        <v>10.15</v>
+      </c>
+      <c r="I24" s="4">
+        <v>3.12</v>
+      </c>
+      <c r="J24" s="4">
+        <v>1.05</v>
+      </c>
+      <c r="K24" s="4">
+        <v>0.74</v>
+      </c>
+      <c r="L24" s="4">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>87</v>
+      </c>
+      <c r="B25" s="4">
+        <v>48.01</v>
+      </c>
+      <c r="C25" s="4">
+        <v>4.17</v>
+      </c>
+      <c r="D25" s="4">
+        <v>13.25</v>
+      </c>
+      <c r="E25" s="4">
+        <v>13.39</v>
+      </c>
+      <c r="F25" s="4">
+        <v>0.23</v>
+      </c>
+      <c r="G25" s="4">
+        <v>4.8099999999999996</v>
+      </c>
+      <c r="H25" s="4">
+        <v>9.57</v>
+      </c>
+      <c r="I25" s="4">
+        <v>3.47</v>
+      </c>
+      <c r="J25" s="4">
+        <v>1.42</v>
+      </c>
+      <c r="K25" s="4">
+        <v>0.86</v>
+      </c>
+      <c r="L25" s="4">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="4"/>
+      <c r="J26" s="4"/>
+      <c r="K26" s="4"/>
+      <c r="L26" s="4"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
+      <c r="I27" s="4"/>
+      <c r="J27" s="4"/>
+      <c r="K27" s="4"/>
+      <c r="L27" s="4"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
+      <c r="H28" s="4"/>
+      <c r="I28" s="4"/>
+      <c r="J28" s="4"/>
+      <c r="K28" s="4"/>
+      <c r="L28" s="4"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="4"/>
+      <c r="I29" s="4"/>
+      <c r="J29" s="4"/>
+      <c r="K29" s="4"/>
+      <c r="L29" s="4"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED9F8352-1565-40C8-9519-00B6A46B7005}">
+  <dimension ref="A1:K16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:11" ht="42" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B2">
+        <v>65.5</v>
+      </c>
+      <c r="D2">
+        <v>19.600000000000001</v>
+      </c>
+      <c r="E2">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0.75</v>
+      </c>
+      <c r="I2">
+        <v>4.8099999999999996</v>
+      </c>
+      <c r="J2">
+        <v>9.36</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B3">
+        <v>65.400000000000006</v>
+      </c>
+      <c r="D3">
+        <v>19.399999999999999</v>
+      </c>
+      <c r="E3">
+        <v>0.05</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0.59</v>
+      </c>
+      <c r="I3">
+        <v>3.13</v>
+      </c>
+      <c r="J3">
+        <v>11.5</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B4">
+        <v>64.599999999999994</v>
+      </c>
+      <c r="D4">
+        <v>18.8</v>
+      </c>
+      <c r="E4">
+        <v>0.09</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0.39</v>
+      </c>
+      <c r="I4">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="J4">
+        <v>14.8</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B5">
+        <v>61.8</v>
+      </c>
+      <c r="D5">
+        <v>19.2</v>
+      </c>
+      <c r="E5">
+        <v>0.51</v>
+      </c>
+      <c r="G5">
+        <v>0.03</v>
+      </c>
+      <c r="H5">
+        <v>0.66</v>
+      </c>
+      <c r="I5">
+        <v>1.71</v>
+      </c>
+      <c r="J5">
+        <v>12.9</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>93</v>
+      </c>
+      <c r="B6">
+        <v>65.099999999999994</v>
+      </c>
+      <c r="D6">
+        <v>19.2</v>
+      </c>
+      <c r="E6">
+        <v>0.05</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0.36</v>
+      </c>
+      <c r="I6">
+        <v>2.87</v>
+      </c>
+      <c r="J6">
+        <v>12.6</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>94</v>
+      </c>
+      <c r="B7">
+        <v>65</v>
+      </c>
+      <c r="D7">
+        <v>19.2</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0.35</v>
+      </c>
+      <c r="I7">
+        <v>2.5099999999999998</v>
+      </c>
+      <c r="J7">
+        <v>12.8</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>95</v>
+      </c>
+      <c r="B8">
+        <v>64.900000000000006</v>
+      </c>
+      <c r="D8">
+        <v>19.3</v>
+      </c>
+      <c r="E8">
+        <v>0.06</v>
+      </c>
+      <c r="G8">
+        <v>0.03</v>
+      </c>
+      <c r="H8">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="I8">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="J8">
+        <v>13.3</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>96</v>
+      </c>
+      <c r="B9">
+        <v>64.900000000000006</v>
+      </c>
+      <c r="D9">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0.17</v>
+      </c>
+      <c r="I9">
+        <v>3.02</v>
+      </c>
+      <c r="J9">
+        <v>12.1</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>97</v>
+      </c>
+      <c r="B10">
+        <v>66</v>
+      </c>
+      <c r="D10">
+        <v>18.899999999999999</v>
+      </c>
+      <c r="E10">
+        <v>0.05</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0.18</v>
+      </c>
+      <c r="I10">
+        <v>3.73</v>
+      </c>
+      <c r="J10">
+        <v>11.3</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>98</v>
+      </c>
+      <c r="B11">
+        <v>66</v>
+      </c>
+      <c r="D11">
+        <v>19.2</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0.18</v>
+      </c>
+      <c r="I11">
+        <v>4.3099999999999996</v>
+      </c>
+      <c r="J11">
+        <v>10.4</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>99</v>
+      </c>
+      <c r="B12">
+        <v>65.5</v>
+      </c>
+      <c r="D12">
+        <v>18.899999999999999</v>
+      </c>
+      <c r="E12">
+        <v>0.11</v>
+      </c>
+      <c r="G12">
+        <v>0.04</v>
+      </c>
+      <c r="H12">
+        <v>0.17</v>
+      </c>
+      <c r="I12">
+        <v>2.58</v>
+      </c>
+      <c r="J12">
+        <v>12.5</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>100</v>
+      </c>
+      <c r="B13">
+        <v>65.3</v>
+      </c>
+      <c r="D13">
+        <v>18.899999999999999</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0.2</v>
+      </c>
+      <c r="I13">
+        <v>3.54</v>
+      </c>
+      <c r="J13">
+        <v>10.9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>101</v>
+      </c>
+      <c r="B14">
+        <v>66.400000000000006</v>
+      </c>
+      <c r="D14">
+        <v>18.8</v>
+      </c>
+      <c r="E14">
+        <v>0.12</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0.25</v>
+      </c>
+      <c r="I14">
+        <v>3.57</v>
+      </c>
+      <c r="J14">
+        <v>11.3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>102</v>
+      </c>
+      <c r="B15">
+        <v>66</v>
+      </c>
+      <c r="D15">
+        <v>18.7</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="I15">
+        <v>2.48</v>
+      </c>
+      <c r="J15">
+        <v>12.7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>103</v>
+      </c>
+      <c r="B16">
+        <v>65.900000000000006</v>
+      </c>
+      <c r="D16">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="E16">
+        <v>0.11</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>0.1</v>
+      </c>
+      <c r="I16">
+        <v>2.54</v>
+      </c>
+      <c r="J16">
+        <v>12.7</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D10DCCC4-E34B-4314-97D3-E2973609E9EF}">
+  <dimension ref="A1:L16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:12" ht="28.2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>61.71</v>
+      </c>
+      <c r="C2">
+        <v>0.45</v>
+      </c>
+      <c r="D2">
+        <v>18.559999999999999</v>
+      </c>
+      <c r="E2">
+        <v>3.17</v>
+      </c>
+      <c r="F2">
+        <v>0.27</v>
+      </c>
+      <c r="G2">
+        <v>0.23</v>
+      </c>
+      <c r="H2">
+        <v>1.64</v>
+      </c>
+      <c r="I2">
+        <v>6.11</v>
+      </c>
+      <c r="J2">
+        <v>7.09</v>
+      </c>
+      <c r="K2">
+        <v>0.02</v>
+      </c>
+      <c r="L2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>61.71</v>
+      </c>
+      <c r="C3">
+        <v>0.45</v>
+      </c>
+      <c r="D3">
+        <v>18.559999999999999</v>
+      </c>
+      <c r="E3">
+        <v>3.17</v>
+      </c>
+      <c r="F3">
+        <v>0.27</v>
+      </c>
+      <c r="G3">
+        <v>0.23</v>
+      </c>
+      <c r="H3">
+        <v>1.64</v>
+      </c>
+      <c r="I3">
+        <v>6.11</v>
+      </c>
+      <c r="J3">
+        <v>7.09</v>
+      </c>
+      <c r="K3">
+        <v>0.02</v>
+      </c>
+      <c r="L3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>62.71</v>
+      </c>
+      <c r="C4">
+        <v>0.45</v>
+      </c>
+      <c r="D4">
+        <v>18.559999999999999</v>
+      </c>
+      <c r="E4">
+        <v>3.17</v>
+      </c>
+      <c r="F4">
+        <v>0.27</v>
+      </c>
+      <c r="G4">
+        <v>0.23</v>
+      </c>
+      <c r="H4">
+        <v>1.64</v>
+      </c>
+      <c r="I4">
+        <v>6.11</v>
+      </c>
+      <c r="J4">
+        <v>6.09</v>
+      </c>
+      <c r="K4">
+        <v>0.02</v>
+      </c>
+      <c r="L4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>62.71</v>
+      </c>
+      <c r="C5">
+        <v>0.45</v>
+      </c>
+      <c r="D5">
+        <v>18.559999999999999</v>
+      </c>
+      <c r="E5">
+        <v>3.17</v>
+      </c>
+      <c r="F5">
+        <v>0.27</v>
+      </c>
+      <c r="G5">
+        <v>0.23</v>
+      </c>
+      <c r="H5">
+        <v>1.64</v>
+      </c>
+      <c r="I5">
+        <v>6.11</v>
+      </c>
+      <c r="J5">
+        <v>6.09</v>
+      </c>
+      <c r="K5">
+        <v>0.02</v>
+      </c>
+      <c r="L5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>62.71</v>
+      </c>
+      <c r="C6">
+        <v>0.45</v>
+      </c>
+      <c r="D6">
+        <v>18.559999999999999</v>
+      </c>
+      <c r="E6">
+        <v>3.17</v>
+      </c>
+      <c r="F6">
+        <v>0.27</v>
+      </c>
+      <c r="G6">
+        <v>0.23</v>
+      </c>
+      <c r="H6">
+        <v>1.64</v>
+      </c>
+      <c r="I6">
+        <v>6.11</v>
+      </c>
+      <c r="J6">
+        <v>6.09</v>
+      </c>
+      <c r="K6">
+        <v>0.02</v>
+      </c>
+      <c r="L6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>62.71</v>
+      </c>
+      <c r="C7">
+        <v>0.45</v>
+      </c>
+      <c r="D7">
+        <v>18.559999999999999</v>
+      </c>
+      <c r="E7">
+        <v>3.17</v>
+      </c>
+      <c r="F7">
+        <v>0.27</v>
+      </c>
+      <c r="G7">
+        <v>0.23</v>
+      </c>
+      <c r="H7">
+        <v>1.64</v>
+      </c>
+      <c r="I7">
+        <v>6.11</v>
+      </c>
+      <c r="J7">
+        <v>6.09</v>
+      </c>
+      <c r="K7">
+        <v>0.02</v>
+      </c>
+      <c r="L7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>62.71</v>
+      </c>
+      <c r="C8">
+        <v>0.45</v>
+      </c>
+      <c r="D8">
+        <v>18.559999999999999</v>
+      </c>
+      <c r="E8">
+        <v>3.17</v>
+      </c>
+      <c r="F8">
+        <v>0.27</v>
+      </c>
+      <c r="G8">
+        <v>0.23</v>
+      </c>
+      <c r="H8">
+        <v>1.64</v>
+      </c>
+      <c r="I8">
+        <v>6.11</v>
+      </c>
+      <c r="J8">
+        <v>6.09</v>
+      </c>
+      <c r="K8">
+        <v>0.02</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>62.71</v>
+      </c>
+      <c r="C9">
+        <v>0.45</v>
+      </c>
+      <c r="D9">
+        <v>18.559999999999999</v>
+      </c>
+      <c r="E9">
+        <v>3.17</v>
+      </c>
+      <c r="F9">
+        <v>0.27</v>
+      </c>
+      <c r="G9">
+        <v>0.23</v>
+      </c>
+      <c r="H9">
+        <v>1.64</v>
+      </c>
+      <c r="I9">
+        <v>6.11</v>
+      </c>
+      <c r="J9">
+        <v>6.09</v>
+      </c>
+      <c r="K9">
+        <v>0.02</v>
+      </c>
+      <c r="L9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>62.71</v>
+      </c>
+      <c r="C10">
+        <v>0.45</v>
+      </c>
+      <c r="D10">
+        <v>18.559999999999999</v>
+      </c>
+      <c r="E10">
+        <v>3.17</v>
+      </c>
+      <c r="F10">
+        <v>0.27</v>
+      </c>
+      <c r="G10">
+        <v>0.23</v>
+      </c>
+      <c r="H10">
+        <v>1.64</v>
+      </c>
+      <c r="I10">
+        <v>6.11</v>
+      </c>
+      <c r="J10">
+        <v>6.09</v>
+      </c>
+      <c r="K10">
+        <v>0.02</v>
+      </c>
+      <c r="L10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>11</v>
+      </c>
+      <c r="B11">
+        <v>63.71</v>
+      </c>
+      <c r="C11">
+        <v>0.45</v>
+      </c>
+      <c r="D11">
+        <v>18.559999999999999</v>
+      </c>
+      <c r="E11">
+        <v>3.17</v>
+      </c>
+      <c r="F11">
+        <v>0.27</v>
+      </c>
+      <c r="G11">
+        <v>0.23</v>
+      </c>
+      <c r="H11">
+        <v>1.64</v>
+      </c>
+      <c r="I11">
+        <v>5.1100000000000003</v>
+      </c>
+      <c r="J11">
+        <v>6.09</v>
+      </c>
+      <c r="K11">
+        <v>0.02</v>
+      </c>
+      <c r="L11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>12</v>
+      </c>
+      <c r="B12">
+        <v>63.71</v>
+      </c>
+      <c r="C12">
+        <v>0.45</v>
+      </c>
+      <c r="D12">
+        <v>18.559999999999999</v>
+      </c>
+      <c r="E12">
+        <v>3.17</v>
+      </c>
+      <c r="F12">
+        <v>0.27</v>
+      </c>
+      <c r="G12">
+        <v>0.23</v>
+      </c>
+      <c r="H12">
+        <v>1.64</v>
+      </c>
+      <c r="I12">
+        <v>5.1100000000000003</v>
+      </c>
+      <c r="J12">
+        <v>6.09</v>
+      </c>
+      <c r="K12">
+        <v>0.02</v>
+      </c>
+      <c r="L12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>13</v>
+      </c>
+      <c r="B13">
+        <v>63.71</v>
+      </c>
+      <c r="C13">
+        <v>0.45</v>
+      </c>
+      <c r="D13">
+        <v>18.559999999999999</v>
+      </c>
+      <c r="E13">
+        <v>3.17</v>
+      </c>
+      <c r="F13">
+        <v>0.27</v>
+      </c>
+      <c r="G13">
+        <v>0.23</v>
+      </c>
+      <c r="H13">
+        <v>1.64</v>
+      </c>
+      <c r="I13">
+        <v>5.1100000000000003</v>
+      </c>
+      <c r="J13">
+        <v>6.09</v>
+      </c>
+      <c r="K13">
+        <v>0.02</v>
+      </c>
+      <c r="L13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>14</v>
+      </c>
+      <c r="B14">
+        <v>63.71</v>
+      </c>
+      <c r="C14">
+        <v>0.45</v>
+      </c>
+      <c r="D14">
+        <v>18.559999999999999</v>
+      </c>
+      <c r="E14">
+        <v>3.17</v>
+      </c>
+      <c r="F14">
+        <v>0.27</v>
+      </c>
+      <c r="G14">
+        <v>0.23</v>
+      </c>
+      <c r="H14">
+        <v>1.64</v>
+      </c>
+      <c r="I14">
+        <v>5.1100000000000003</v>
+      </c>
+      <c r="J14">
+        <v>6.09</v>
+      </c>
+      <c r="K14">
+        <v>0.02</v>
+      </c>
+      <c r="L14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>15</v>
+      </c>
+      <c r="B15">
+        <v>63.71</v>
+      </c>
+      <c r="C15">
+        <v>0.45</v>
+      </c>
+      <c r="D15">
+        <v>18.559999999999999</v>
+      </c>
+      <c r="E15">
+        <v>3.17</v>
+      </c>
+      <c r="F15">
+        <v>0.27</v>
+      </c>
+      <c r="G15">
+        <v>0.23</v>
+      </c>
+      <c r="H15">
+        <v>1.64</v>
+      </c>
+      <c r="I15">
+        <v>5.1100000000000003</v>
+      </c>
+      <c r="J15">
+        <v>6.09</v>
+      </c>
+      <c r="K15">
+        <v>0.02</v>
+      </c>
+      <c r="L15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>16</v>
+      </c>
+      <c r="B16">
+        <v>63.71</v>
+      </c>
+      <c r="C16">
+        <v>0.45</v>
+      </c>
+      <c r="D16">
+        <v>18.559999999999999</v>
+      </c>
+      <c r="E16">
+        <v>3.17</v>
+      </c>
+      <c r="F16">
+        <v>0.27</v>
+      </c>
+      <c r="G16">
+        <v>0.23</v>
+      </c>
+      <c r="H16">
+        <v>1.64</v>
+      </c>
+      <c r="I16">
+        <v>5.1100000000000003</v>
+      </c>
+      <c r="J16">
+        <v>6.09</v>
+      </c>
+      <c r="K16">
+        <v>0.02</v>
+      </c>
+      <c r="L16">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>